<commit_message>
Vista de Truck Details
</commit_message>
<xml_diff>
--- a/Documentacion/Roles table.xlsx
+++ b/Documentacion/Roles table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Axis\Axis website\axis\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>Roles</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>CUANDO EL FIELD OPS RECHAZA, GUARDAR COMENTARIO</t>
-  </si>
-  <si>
-    <t>STATUS BY TRUCKS DETAILS</t>
-  </si>
-  <si>
-    <t>PENDING RENT</t>
   </si>
 </sst>
 </file>
@@ -340,10 +334,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -942,10 +936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E33"/>
+  <dimension ref="B3:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,10 +949,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>52</v>
       </c>
@@ -1025,7 +1019,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D13" t="s">
@@ -1053,7 +1047,7 @@
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1081,7 +1075,7 @@
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="8" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1115,16 +1109,6 @@
       </c>
       <c r="D29" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>